<commit_message>
Ajustes segun documento MSEXCEL
</commit_message>
<xml_diff>
--- a/Docs/TIEMPOS PROYECTO DEMO.xlsx
+++ b/Docs/TIEMPOS PROYECTO DEMO.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\DelphiXE\Apps\ZEOSLIB\Prod\ZEOSLIB_08MasQueImpresos\Docs\"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Horas</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>2021-10-17</t>
+  </si>
+  <si>
+    <t>2021-10-19</t>
   </si>
 </sst>
 </file>
@@ -66,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -79,18 +82,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -143,7 +134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -155,8 +146,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -506,10 +495,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L45"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="B2:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -558,7 +548,7 @@
         <v>120</v>
       </c>
       <c r="J3">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -592,11 +582,11 @@
       </c>
       <c r="J4" s="10">
         <f>I4*J$3%</f>
-        <v>334800</v>
+        <v>372000</v>
       </c>
       <c r="K4" s="10">
         <f>I4-J4</f>
-        <v>37200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -630,11 +620,11 @@
       </c>
       <c r="J5" s="10">
         <f>I5*J$3%</f>
-        <v>419040</v>
+        <v>465600</v>
       </c>
       <c r="K5" s="10">
         <f>I5-J5</f>
-        <v>46560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -651,7 +641,7 @@
         <v>0.71111111111111114</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6:F7" si="8">E6-D6</f>
+        <f t="shared" ref="F6:F8" si="8">E6-D6</f>
         <v>0.12777777777777777</v>
       </c>
       <c r="G6" s="3">
@@ -668,11 +658,11 @@
       </c>
       <c r="J6" s="10">
         <f>I6*J$3%</f>
-        <v>397440</v>
+        <v>441600</v>
       </c>
       <c r="K6" s="10">
         <f>I6-J6</f>
-        <v>44160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -693,7 +683,7 @@
         <v>6.6666666666666652E-2</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" ref="G7" si="12">(HOUR(F7)*60)+MINUTE(F7)</f>
+        <f t="shared" ref="G7:G8" si="12">(HOUR(F7)*60)+MINUTE(F7)</f>
         <v>96</v>
       </c>
       <c r="H7" s="3">
@@ -706,28 +696,88 @@
       </c>
       <c r="J7" s="10">
         <f>I7*J$3%</f>
-        <v>207360</v>
+        <v>230400</v>
       </c>
       <c r="K7" s="10">
         <f>I7-J7</f>
-        <v>23040</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="8"/>
+        <v>0.125</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="12"/>
+        <v>180</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" ref="H8" si="15">(H$3/60)*(I$3/100)</f>
+        <v>2400</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" ref="I8" si="16">G8*H8</f>
+        <v>432000</v>
+      </c>
+      <c r="J8" s="10">
+        <f>I8*J$3%</f>
+        <v>432000</v>
+      </c>
+      <c r="K8" s="10">
+        <f>I8-J8</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.8125</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.88680555555555562</v>
+      </c>
+      <c r="F9" s="4">
+        <f t="shared" ref="F9" si="17">E9-D9</f>
+        <v>7.4305555555555625E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" ref="G9" si="18">(HOUR(F9)*60)+MINUTE(F9)</f>
+        <v>107</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" ref="H9" si="19">(H$3/60)*(I$3/100)</f>
+        <v>2400</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" ref="I9" si="20">G9*H9</f>
+        <v>256800</v>
+      </c>
+      <c r="J9" s="10">
+        <f>I9*J$3%</f>
+        <v>256800</v>
+      </c>
+      <c r="K9" s="10">
+        <f>I9-J9</f>
+        <v>0</v>
+      </c>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -746,130 +796,40 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="11"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="11"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G18" s="9"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G19" s="9"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G20" s="9"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G21" s="9"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G22" s="9"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G23" s="9"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
-      <c r="F42" s="13">
-        <f>SUM(F4:F40)</f>
-        <v>0.43680555555555561</v>
-      </c>
-      <c r="G42" s="7">
-        <f>SUM(G3:G40)</f>
-        <v>629</v>
-      </c>
-      <c r="H42" s="8" t="s">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B30" s="6"/>
+      <c r="F30" s="11">
+        <f>SUM(F4:F28)</f>
+        <v>0.63611111111111129</v>
+      </c>
+      <c r="G30" s="7">
+        <f>SUM(G3:G28)</f>
+        <v>916</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="7">
-        <f>SUM(I3:I40)</f>
-        <v>1509720</v>
-      </c>
-      <c r="J42" s="7">
-        <f>SUM(J3:J40)</f>
-        <v>1358730</v>
-      </c>
-      <c r="K42" s="7">
-        <f>SUM(K3:K40)</f>
-        <v>150960</v>
-      </c>
-      <c r="L42" s="7">
-        <f>SUM(L3:L40)</f>
+      <c r="I30" s="7">
+        <f>SUM(I3:I28)</f>
+        <v>2198520</v>
+      </c>
+      <c r="J30" s="7">
+        <f>SUM(J3:J28)</f>
+        <v>2198500</v>
+      </c>
+      <c r="K30" s="7">
+        <f>SUM(K3:K28)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="F45" s="4">
-        <f>F42/8</f>
-        <v>5.4600694444444452E-2</v>
+      <c r="L30" s="7">
+        <f>SUM(L3:L28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="4">
+        <f>F30/8</f>
+        <v>7.9513888888888912E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>